<commit_message>
[Swapnil] Add :Check for duplicate records during adding records
</commit_message>
<xml_diff>
--- a/RetrievedContacts.xlsx
+++ b/RetrievedContacts.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="34">
   <si>
     <t>first_name</t>
   </si>
@@ -37,12 +37,6 @@
     <t>phone_number</t>
   </si>
   <si>
-    <t>Book_Name</t>
-  </si>
-  <si>
-    <t>Contact_Type</t>
-  </si>
-  <si>
     <t>Sue</t>
   </si>
   <si>
@@ -58,15 +52,6 @@
     <t>IL</t>
   </si>
   <si>
-    <t>MyBook</t>
-  </si>
-  <si>
-    <t>Friends</t>
-  </si>
-  <si>
-    <t>Family</t>
-  </si>
-  <si>
     <t>Mike</t>
   </si>
   <si>
@@ -91,9 +76,6 @@
     <t>100 5th Ave.</t>
   </si>
   <si>
-    <t>Professional</t>
-  </si>
-  <si>
     <t>Meg</t>
   </si>
   <si>
@@ -116,6 +98,24 @@
   </si>
   <si>
     <t>500 South St.</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>sueblack@gmail.com</t>
+  </si>
+  <si>
+    <t>mikeybrown@gmail.com</t>
+  </si>
+  <si>
+    <t>lizwhite@yahoo.com</t>
+  </si>
+  <si>
+    <t>megsteph@gmaco.com</t>
+  </si>
+  <si>
+    <t>johngray@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -457,13 +457,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I7"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J6" sqref="A1:J6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -486,27 +488,24 @@
         <v>6</v>
       </c>
       <c r="H1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="B2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="C2" t="s">
         <v>9</v>
       </c>
-      <c r="B2" t="s">
+      <c r="D2" t="s">
         <v>10</v>
       </c>
-      <c r="C2" t="s">
+      <c r="E2" t="s">
         <v>11</v>
-      </c>
-      <c r="D2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E2" t="s">
-        <v>13</v>
       </c>
       <c r="F2">
         <v>60605</v>
@@ -515,42 +514,36 @@
         <v>3889233120</v>
       </c>
       <c r="H2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" t="s">
         <v>14</v>
       </c>
-      <c r="I2" t="s">
+      <c r="D3" t="s">
         <v>15</v>
       </c>
+      <c r="E3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3">
+        <v>10011</v>
+      </c>
+      <c r="G3">
+        <v>8832322103</v>
+      </c>
+      <c r="H3" t="s">
+        <v>30</v>
+      </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F3">
-        <v>60605</v>
-      </c>
-      <c r="G3">
-        <v>3889233120</v>
-      </c>
-      <c r="H3" t="s">
-        <v>14</v>
-      </c>
-      <c r="I3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>17</v>
       </c>
@@ -561,109 +554,71 @@
         <v>19</v>
       </c>
       <c r="D4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4">
+        <v>10012</v>
+      </c>
+      <c r="G4">
+        <v>8043232213</v>
+      </c>
+      <c r="H4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>20</v>
       </c>
-      <c r="E4" t="s">
+      <c r="B5" t="s">
         <v>21</v>
       </c>
-      <c r="F4">
-        <v>10011</v>
-      </c>
-      <c r="G4">
-        <v>8832322103</v>
-      </c>
-      <c r="H4" t="s">
-        <v>14</v>
-      </c>
-      <c r="I4" t="s">
-        <v>15</v>
+      <c r="C5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E5" t="s">
+        <v>24</v>
+      </c>
+      <c r="F5">
+        <v>80204</v>
+      </c>
+      <c r="G5">
+        <v>7884440432</v>
+      </c>
+      <c r="H5" t="s">
+        <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B5" t="s">
-        <v>23</v>
-      </c>
-      <c r="C5" t="s">
-        <v>24</v>
-      </c>
-      <c r="D5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E5" t="s">
-        <v>21</v>
-      </c>
-      <c r="F5">
-        <v>10012</v>
-      </c>
-      <c r="G5">
-        <v>8043232213</v>
-      </c>
-      <c r="H5" t="s">
-        <v>14</v>
-      </c>
-      <c r="I5" t="s">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="B6" t="s">
         <v>26</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>27</v>
       </c>
-      <c r="C6" t="s">
-        <v>28</v>
-      </c>
       <c r="D6" t="s">
-        <v>29</v>
+        <v>10</v>
       </c>
       <c r="E6" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="F6">
-        <v>80204</v>
+        <v>60605</v>
       </c>
       <c r="G6">
-        <v>7884440432</v>
+        <v>8334432122</v>
       </c>
       <c r="H6" t="s">
-        <v>14</v>
-      </c>
-      <c r="I6" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>31</v>
-      </c>
-      <c r="B7" t="s">
-        <v>32</v>
-      </c>
-      <c r="C7" t="s">
         <v>33</v>
-      </c>
-      <c r="D7" t="s">
-        <v>12</v>
-      </c>
-      <c r="E7" t="s">
-        <v>13</v>
-      </c>
-      <c r="F7">
-        <v>60605</v>
-      </c>
-      <c r="G7">
-        <v>8334432122</v>
-      </c>
-      <c r="H7" t="s">
-        <v>14</v>
-      </c>
-      <c r="I7" t="s">
-        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>